<commit_message>
vahed 14 va 1 toman seraydar
</commit_message>
<xml_diff>
--- a/Building-Management .xlsx
+++ b/Building-Management .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohsen\Documents\Building-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C748CF3-9A26-4782-8464-7A0159333A9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA0C17B-898C-47A4-B0F3-3E8775D80F38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR606"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="B28" s="5">
         <f>975000+B23+G23+K23+O23+T23+Y23+AD23+AH23+AL23+AQ23+AU23+AY23+BC23+BG23+BK23+BP23+B53+F53+J53</f>
-        <v>3771900</v>
+        <v>2801900</v>
       </c>
       <c r="C28" s="5"/>
       <c r="AC28" s="21"/>
@@ -4853,7 +4853,7 @@
         <v>11</v>
       </c>
       <c r="H33" s="40">
-        <v>1870000</v>
+        <v>2000000</v>
       </c>
       <c r="I33" s="30" t="s">
         <v>7</v>
@@ -4862,7 +4862,9 @@
       <c r="K33" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L33" s="31"/>
+      <c r="L33" s="31">
+        <v>1000000</v>
+      </c>
       <c r="AC33" s="21"/>
       <c r="AD33" s="21"/>
       <c r="AE33" s="21"/>
@@ -5232,7 +5234,9 @@
       <c r="I45" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J45" s="31"/>
+      <c r="J45" s="31">
+        <v>160000</v>
+      </c>
       <c r="K45" s="30"/>
       <c r="L45" s="31"/>
       <c r="AC45" s="21"/>
@@ -5387,21 +5391,21 @@
       </c>
       <c r="H51" s="40">
         <f>SUM(H32:H50)</f>
-        <v>2564900</v>
+        <v>2694900</v>
       </c>
       <c r="I51" s="32" t="s">
         <v>32</v>
       </c>
       <c r="J51" s="31">
         <f>SUM(J32:J48)</f>
-        <v>160000</v>
+        <v>320000</v>
       </c>
       <c r="K51" s="32" t="s">
         <v>33</v>
       </c>
       <c r="L51" s="31">
         <f>SUM(L32:L50)</f>
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="AC51" s="21"/>
       <c r="AD51" s="21"/>
@@ -5441,7 +5445,7 @@
       </c>
       <c r="F53" s="40">
         <f>(F51-H51)</f>
-        <v>155100</v>
+        <v>25100</v>
       </c>
       <c r="G53" s="41"/>
       <c r="H53" s="40"/>
@@ -5450,7 +5454,7 @@
       </c>
       <c r="J53" s="31">
         <f>(J51-L51)</f>
-        <v>160000</v>
+        <v>-680000</v>
       </c>
       <c r="K53" s="32"/>
       <c r="L53" s="31"/>

</xml_diff>